<commit_message>
El generador está funcionando bien, pero quedan algunos detallitos que solucionar
</commit_message>
<xml_diff>
--- a/rubroRegion.xlsx
+++ b/rubroRegion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,18 +485,16 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Equipos, accesorios y suministros de oficina</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>904.5643009310008</v>
+        <v>901745.342027444</v>
       </c>
       <c r="F2" t="n">
-        <v>800000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>22.11416714495812</v>
-      </c>
+        <v>755558432.84</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>0</v>
       </c>
@@ -511,30 +509,24 @@
       <c r="B3" t="n">
         <v>2023</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Antofagasta</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Servicios de limpieza industrial</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>69759372.5955651</v>
+        <v>619549.5905107583</v>
       </c>
       <c r="F3" t="n">
-        <v>57387250025</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1592490.162199131</v>
-      </c>
+        <v>510549401.65</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -544,30 +536,24 @@
       <c r="B4" t="n">
         <v>2023</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Antofagasta</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>37365878.47939286</v>
+        <v>279168.0421732903</v>
       </c>
       <c r="F4" t="n">
-        <v>31775755713.11144</v>
-      </c>
-      <c r="G4" t="n">
-        <v>881125.6060268474</v>
-      </c>
+        <v>232866300.68</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -577,30 +563,24 @@
       <c r="B5" t="n">
         <v>2023</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Antofagasta</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Obras MINVU</t>
+          <t>Servicios de transporte, almacenaje y correo</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>25665374.41055844</v>
+        <v>252417.4300486843</v>
       </c>
       <c r="F5" t="n">
-        <v>20807430211</v>
-      </c>
-      <c r="G5" t="n">
-        <v>583149.9534718788</v>
-      </c>
+        <v>212712186</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -610,30 +590,24 @@
       <c r="B6" t="n">
         <v>2023</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Antofagasta</t>
-        </is>
-      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Servicios de limpieza industrial</t>
+          <t>Artículos eléctricos y de iluminación</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>22168240.57605305</v>
+        <v>185353.64600234</v>
       </c>
       <c r="F6" t="n">
-        <v>18595364133.02091</v>
-      </c>
-      <c r="G6" t="n">
-        <v>518143.4743053182</v>
-      </c>
+        <v>162446749</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -650,23 +624,21 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Salud, servicios sanitarios y alimentación</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>19309635.37900426</v>
+        <v>200782582.7296285</v>
       </c>
       <c r="F7" t="n">
-        <v>16175388490.43118</v>
-      </c>
-      <c r="G7" t="n">
-        <v>449741.9537931414</v>
-      </c>
+        <v>172210606470.1</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -678,28 +650,26 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Araucanía</t>
+          <t>Antofagasta</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>72405165.13124916</v>
+        <v>43525675.8456754</v>
       </c>
       <c r="F8" t="n">
-        <v>61888054669.01922</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1714866.586777889</v>
-      </c>
+        <v>37161120531.35535</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -711,28 +681,26 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Araucanía</t>
+          <t>Antofagasta</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Servicios de limpieza industrial</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>59824667.77713408</v>
+        <v>28528175.3848198</v>
       </c>
       <c r="F9" t="n">
-        <v>49755786719.97237</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1385957.820562994</v>
-      </c>
+        <v>24130276882.70694</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -744,28 +712,26 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Araucanía</t>
+          <t>Antofagasta</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+          <t>Obras MINVU</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>57993360.33034196</v>
+        <v>25665374.41055844</v>
       </c>
       <c r="F10" t="n">
-        <v>48411609228.43455</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1349504.469346422</v>
-      </c>
+        <v>20807430211</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -777,28 +743,26 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Araucanía</t>
+          <t>Antofagasta</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>46823237.19824554</v>
+        <v>22941684.16735266</v>
       </c>
       <c r="F11" t="n">
-        <v>39138488868.24046</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1090752.410025413</v>
-      </c>
+        <v>19330580572.54248</v>
+      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -813,25 +777,21 @@
           <t>Araucanía</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Servicios de transporte, almacenaje y correo</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>41032530.19648424</v>
+        <v>116133915.7099773</v>
       </c>
       <c r="F12" t="n">
-        <v>34165148678.24831</v>
+        <v>96705116160</v>
       </c>
       <c r="G12" t="n">
-        <v>951239.1510178581</v>
+        <v>2681005.769840984</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -843,28 +803,26 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Arica y Parinacota</t>
+          <t>Araucanía</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>70951753.56151588</v>
+        <v>64125357.10944952</v>
       </c>
       <c r="F13" t="n">
-        <v>62830074935</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1722742.160522497</v>
-      </c>
+        <v>53517744694.78053</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -876,28 +834,26 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Arica y Parinacota</t>
+          <t>Araucanía</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Servicios de limpieza industrial</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>19711397.99516376</v>
+        <v>63787457.90708901</v>
       </c>
       <c r="F14" t="n">
-        <v>16075563603.40473</v>
-      </c>
-      <c r="G14" t="n">
-        <v>446675.9946439902</v>
-      </c>
+        <v>53485522347.2868</v>
+      </c>
+      <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -909,7 +865,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Arica y Parinacota</t>
+          <t>Araucanía</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -918,19 +874,17 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>18144078.40322741</v>
+        <v>54422704.98659359</v>
       </c>
       <c r="F15" t="n">
-        <v>15057697466.03142</v>
-      </c>
-      <c r="G15" t="n">
-        <v>419580.4429625535</v>
-      </c>
+        <v>45855734441.98038</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -942,7 +896,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Arica y Parinacota</t>
+          <t>Araucanía</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -951,19 +905,17 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>10920175.41546245</v>
+        <v>45258967.52201545</v>
       </c>
       <c r="F16" t="n">
-        <v>9029167040.638348</v>
-      </c>
-      <c r="G16" t="n">
-        <v>251831.0272972065</v>
-      </c>
+        <v>37890607898.8496</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -978,25 +930,21 @@
           <t>Arica y Parinacota</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Consultoria</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>9505688.609760471</v>
+        <v>1352270603090615</v>
       </c>
       <c r="F17" t="n">
-        <v>8557796518</v>
+        <v>1.087004945419017e+18</v>
       </c>
       <c r="G17" t="n">
-        <v>235014.3173276998</v>
+        <v>30476785573881.11</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1008,28 +956,26 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Atacama</t>
+          <t>Arica y Parinacota</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Servicios basados en ingeniería, ciencias sociales y tecnología de la información</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>44904776.00820866</v>
+        <v>35654089.69784889</v>
       </c>
       <c r="F18" t="n">
-        <v>37445743399.67721</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1039017.937791309</v>
-      </c>
+        <v>30113570613.80602</v>
+      </c>
+      <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1041,28 +987,26 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Atacama</t>
+          <t>Arica y Parinacota</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Servicios de transporte, almacenaje y correo</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>12000618.47151066</v>
+        <v>21445120.03490136</v>
       </c>
       <c r="F19" t="n">
-        <v>9991545633.37981</v>
-      </c>
-      <c r="G19" t="n">
-        <v>278246.1757160855</v>
-      </c>
+        <v>17842193140.04343</v>
+      </c>
+      <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -1074,28 +1018,26 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Atacama</t>
+          <t>Arica y Parinacota</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Servicios de transporte, almacenaje y correo</t>
+          <t>Servicios de limpieza industrial</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>10777065.88263122</v>
+        <v>20099303.14632814</v>
       </c>
       <c r="F20" t="n">
-        <v>8949995154.088566</v>
-      </c>
-      <c r="G20" t="n">
-        <v>249277.1941725995</v>
-      </c>
+        <v>16413677617.78473</v>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -1107,28 +1049,26 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Atacama</t>
+          <t>Arica y Parinacota</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>8488128.406172631</v>
+        <v>19330050.16764392</v>
       </c>
       <c r="F21" t="n">
-        <v>7185869778.364071</v>
-      </c>
-      <c r="G21" t="n">
-        <v>199753.5673157675</v>
-      </c>
+        <v>16093992591.11241</v>
+      </c>
+      <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -1145,23 +1085,21 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>7687748.583955027</v>
+        <v>54531112.75793689</v>
       </c>
       <c r="F22" t="n">
-        <v>6578095441</v>
-      </c>
-      <c r="G22" t="n">
-        <v>182376.8198501633</v>
-      </c>
+        <v>45862515884.4021</v>
+      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1173,28 +1111,26 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Aysén</t>
+          <t>Atacama</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>67133914.73708832</v>
+        <v>13068163.0374981</v>
       </c>
       <c r="F23" t="n">
-        <v>55351222516</v>
-      </c>
-      <c r="G23" t="n">
-        <v>1557408.603016248</v>
-      </c>
+        <v>10925217940.37981</v>
+      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -1206,28 +1142,26 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Aysén</t>
+          <t>Atacama</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>28571817.10794167</v>
+        <v>12405223.91676243</v>
       </c>
       <c r="F24" t="n">
-        <v>24244403218.35291</v>
-      </c>
-      <c r="G24" t="n">
-        <v>672797.3807979024</v>
-      </c>
+        <v>10611998519.18348</v>
+      </c>
+      <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -1239,7 +1173,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Aysén</t>
+          <t>Atacama</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1248,19 +1182,17 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>12375717.48420958</v>
+        <v>11604608.89120818</v>
       </c>
       <c r="F25" t="n">
-        <v>10352803089.55004</v>
-      </c>
-      <c r="G25" t="n">
-        <v>287948.2947352765</v>
-      </c>
+        <v>9673860675.228569</v>
+      </c>
+      <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -1272,28 +1204,24 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Aysén</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
-        </is>
-      </c>
+          <t>Atacama</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>10001189.44687807</v>
+        <v>8108010.321714605</v>
       </c>
       <c r="F26" t="n">
-        <v>8414405437.181916</v>
+        <v>6923824055</v>
       </c>
       <c r="G26" t="n">
-        <v>234062.4281128414</v>
+        <v>191962.0064127275</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1308,25 +1236,21 @@
           <t>Aysén</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Equipamiento y suministros médicos</t>
-        </is>
-      </c>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>7800148.632654455</v>
+        <v>75181925535215.67</v>
       </c>
       <c r="F27" t="n">
-        <v>6547440428.461759</v>
+        <v>6.266449654996442e+16</v>
       </c>
       <c r="G27" t="n">
-        <v>182170.7944228594</v>
+        <v>1735822490109.256</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1338,28 +1262,26 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Bío-Bío</t>
+          <t>Aysén</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>99610315.54780802</v>
+        <v>31177870.90745586</v>
       </c>
       <c r="F28" t="n">
-        <v>83124579775.20418</v>
-      </c>
-      <c r="G28" t="n">
-        <v>2313186.773817586</v>
-      </c>
+        <v>26521149604.0243</v>
+      </c>
+      <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1371,28 +1293,26 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bío-Bío</t>
+          <t>Aysén</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Servicios de transporte, almacenaje y correo</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>99034961.81474052</v>
+        <v>14003763.78279521</v>
       </c>
       <c r="F29" t="n">
-        <v>83785979341.95575</v>
-      </c>
-      <c r="G29" t="n">
-        <v>2326889.680252589</v>
-      </c>
+        <v>11775102934.55973</v>
+      </c>
+      <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1404,28 +1324,26 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Bío-Bío</t>
+          <t>Aysén</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>52791402.02026006</v>
+        <v>11009973.86117144</v>
       </c>
       <c r="F30" t="n">
-        <v>43243161286</v>
-      </c>
-      <c r="G30" t="n">
-        <v>1205751.69297413</v>
-      </c>
+        <v>9294968316.416376</v>
+      </c>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1437,28 +1355,26 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Bío-Bío</t>
+          <t>Aysén</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Servicios de limpieza industrial</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>49720240.65846659</v>
+        <v>9536607.435378332</v>
       </c>
       <c r="F31" t="n">
-        <v>40963727583.47488</v>
-      </c>
-      <c r="G31" t="n">
-        <v>1141440.442331109</v>
-      </c>
+        <v>8064745659.00032</v>
+      </c>
+      <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -1475,23 +1391,21 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>48796045.03772824</v>
+        <v>116062214.9149046</v>
       </c>
       <c r="F32" t="n">
-        <v>40440187204.24339</v>
-      </c>
-      <c r="G32" t="n">
-        <v>1125969.915611054</v>
-      </c>
+        <v>98668785006.57314</v>
+      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1503,28 +1417,26 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Coquimbo</t>
+          <t>Bío-Bío</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>48062307.86517344</v>
+        <v>110198246.1385839</v>
       </c>
       <c r="F33" t="n">
-        <v>39324837456</v>
-      </c>
-      <c r="G33" t="n">
-        <v>1101346.109914959</v>
-      </c>
+        <v>92384853982.52975</v>
+      </c>
+      <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34">
@@ -1536,28 +1448,26 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Coquimbo</t>
+          <t>Bío-Bío</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>38635183.68888644</v>
+        <v>55556721.0422359</v>
       </c>
       <c r="F34" t="n">
-        <v>32602843549.57549</v>
-      </c>
-      <c r="G34" t="n">
-        <v>907513.508380628</v>
-      </c>
+        <v>46340282395.06536</v>
+      </c>
+      <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
         <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -1569,28 +1479,24 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Coquimbo</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Equipamiento y suministros médicos</t>
-        </is>
-      </c>
+          <t>Bío-Bío</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>36389113.94082711</v>
+        <v>54240121.2510023</v>
       </c>
       <c r="F35" t="n">
-        <v>30293490543.10932</v>
+        <v>44404038953</v>
       </c>
       <c r="G35" t="n">
-        <v>843166.5233937924</v>
+        <v>1238042.772370678</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1602,28 +1508,26 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Coquimbo</t>
+          <t>Bío-Bío</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Servicios de transporte, almacenaje y correo</t>
+          <t>Servicios de limpieza industrial</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>20516949.50275848</v>
+        <v>53342830.59164016</v>
       </c>
       <c r="F36" t="n">
-        <v>17111272001.86536</v>
-      </c>
-      <c r="G36" t="n">
-        <v>476174.2803249512</v>
-      </c>
+        <v>44132044935.6428</v>
+      </c>
+      <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -1638,25 +1542,21 @@
           <t>Coquimbo</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Servicios de limpieza industrial</t>
-        </is>
-      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>16369441.09878701</v>
+        <v>297771937195863.6</v>
       </c>
       <c r="F37" t="n">
-        <v>13876415456.07568</v>
+        <v>2.604412083314865e+17</v>
       </c>
       <c r="G37" t="n">
-        <v>384942.6682883084</v>
+        <v>7102417245230.266</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1668,7 +1568,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Lib. Gral. Bdo. O'Higgins</t>
+          <t>Coquimbo</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1677,19 +1577,17 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>57425848.26882367</v>
+        <v>41633397.43545135</v>
       </c>
       <c r="F38" t="n">
-        <v>48182475629.51656</v>
-      </c>
-      <c r="G38" t="n">
-        <v>1339926.370259461</v>
-      </c>
+        <v>35225171237.5635</v>
+      </c>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
         <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
@@ -1701,28 +1599,26 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Lib. Gral. Bdo. O'Higgins</t>
+          <t>Coquimbo</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>33683590.70389374</v>
+        <v>39688754.07025614</v>
       </c>
       <c r="F39" t="n">
-        <v>28248836777.51088</v>
-      </c>
-      <c r="G39" t="n">
-        <v>787687.7559457625</v>
-      </c>
+        <v>33178669559.64686</v>
+      </c>
+      <c r="G39" t="inlineStr"/>
       <c r="H39" t="n">
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -1734,28 +1630,26 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Lib. Gral. Bdo. O'Higgins</t>
+          <t>Coquimbo</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Servicios de transporte, almacenaje y correo</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>28224334.3793799</v>
+        <v>22735563.36148095</v>
       </c>
       <c r="F40" t="n">
-        <v>23470857995.04953</v>
-      </c>
-      <c r="G40" t="n">
-        <v>653784.5053934368</v>
-      </c>
+        <v>19051480355.64533</v>
+      </c>
+      <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
         <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
@@ -1767,28 +1661,26 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Lib. Gral. Bdo. O'Higgins</t>
+          <t>Coquimbo</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Servicios de transporte, almacenaje y correo</t>
+          <t>Servicios de limpieza industrial</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>23286562.37615285</v>
+        <v>21923195.17128803</v>
       </c>
       <c r="F41" t="n">
-        <v>19367061387.16066</v>
-      </c>
-      <c r="G41" t="n">
-        <v>539219.8102081214</v>
-      </c>
+        <v>18733871908.928</v>
+      </c>
+      <c r="G41" t="inlineStr"/>
       <c r="H41" t="n">
         <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -1805,23 +1697,21 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Servicios de limpieza industrial</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>22276715.99086813</v>
+        <v>63196714.87987141</v>
       </c>
       <c r="F42" t="n">
-        <v>18400981524.75328</v>
-      </c>
-      <c r="G42" t="n">
-        <v>515902.3154080256</v>
-      </c>
+        <v>53210729461.0369</v>
+      </c>
+      <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1833,28 +1723,26 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Los Lagos</t>
+          <t>Lib. Gral. Bdo. O'Higgins</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>98979489.57371847</v>
+        <v>38511999.087263</v>
       </c>
       <c r="F43" t="n">
-        <v>82408477423.92407</v>
-      </c>
-      <c r="G43" t="n">
-        <v>2295368.681430223</v>
-      </c>
+        <v>32445528788.7043</v>
+      </c>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
         <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
@@ -1866,7 +1754,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Los Lagos</t>
+          <t>Lib. Gral. Bdo. O'Higgins</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1875,19 +1763,17 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>45178962.38305318</v>
+        <v>32081165.41547768</v>
       </c>
       <c r="F44" t="n">
-        <v>37799152704.73763</v>
-      </c>
-      <c r="G44" t="n">
-        <v>1051386.241226903</v>
-      </c>
+        <v>26841455077.30179</v>
+      </c>
+      <c r="G44" t="inlineStr"/>
       <c r="H44" t="n">
         <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
@@ -1899,7 +1785,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Los Lagos</t>
+          <t>Lib. Gral. Bdo. O'Higgins</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1908,19 +1794,17 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>28103635.50306795</v>
+        <v>25397943.36118131</v>
       </c>
       <c r="F45" t="n">
-        <v>23411822723.80079</v>
-      </c>
-      <c r="G45" t="n">
-        <v>652566.0329130271</v>
-      </c>
+        <v>21207261273.46177</v>
+      </c>
+      <c r="G45" t="inlineStr"/>
       <c r="H45" t="n">
         <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
@@ -1932,7 +1816,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Los Lagos</t>
+          <t>Lib. Gral. Bdo. O'Higgins</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1941,19 +1825,17 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>24703469.12599881</v>
+        <v>24393372.03552687</v>
       </c>
       <c r="F46" t="n">
-        <v>20317710003.12287</v>
-      </c>
-      <c r="G46" t="n">
-        <v>568075.4771504527</v>
-      </c>
+        <v>20252256439.76813</v>
+      </c>
+      <c r="G46" t="inlineStr"/>
       <c r="H46" t="n">
         <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
@@ -1970,23 +1852,21 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>21556329.2708141</v>
+        <v>123386252.6613988</v>
       </c>
       <c r="F47" t="n">
-        <v>17846209919.9379</v>
-      </c>
-      <c r="G47" t="n">
-        <v>497212.5377816397</v>
-      </c>
+        <v>103754722050.9581</v>
+      </c>
+      <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
         <v>0</v>
       </c>
       <c r="I47" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -1998,28 +1878,26 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Los Ríos</t>
+          <t>Los Lagos</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>88870514.79716723</v>
+        <v>59098560.77217842</v>
       </c>
       <c r="F48" t="n">
-        <v>71645911614.1114</v>
-      </c>
-      <c r="G48" t="n">
-        <v>1997211.793587974</v>
-      </c>
+        <v>49579353199.74539</v>
+      </c>
+      <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
         <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
@@ -2031,28 +1909,26 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Los Ríos</t>
+          <t>Los Lagos</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Servicios de transporte, almacenaje y correo</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>37678667.29859822</v>
+        <v>30572914.56840733</v>
       </c>
       <c r="F49" t="n">
-        <v>31584317385.67822</v>
-      </c>
-      <c r="G49" t="n">
-        <v>877818.2535817946</v>
-      </c>
+        <v>25571536140.43476</v>
+      </c>
+      <c r="G49" t="inlineStr"/>
       <c r="H49" t="n">
         <v>0</v>
       </c>
       <c r="I49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
@@ -2064,28 +1940,26 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Los Ríos</t>
+          <t>Los Lagos</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+          <t>Servicios de limpieza industrial</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>23946416.63420506</v>
+        <v>25730540.22009587</v>
       </c>
       <c r="F50" t="n">
-        <v>20099312190.76742</v>
-      </c>
-      <c r="G50" t="n">
-        <v>559811.5101239822</v>
-      </c>
+        <v>21208058014.67456</v>
+      </c>
+      <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
         <v>0</v>
       </c>
       <c r="I50" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -2097,28 +1971,26 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Los Ríos</t>
+          <t>Los Lagos</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>17911610.2603449</v>
+        <v>24915025.19560209</v>
       </c>
       <c r="F51" t="n">
-        <v>14817893210.03977</v>
-      </c>
-      <c r="G51" t="n">
-        <v>412445.1990067547</v>
-      </c>
+        <v>20783598106.66674</v>
+      </c>
+      <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
         <v>0</v>
       </c>
       <c r="I51" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
@@ -2133,25 +2005,21 @@
           <t>Los Ríos</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Salud, servicios sanitarios y alimentación</t>
-        </is>
-      </c>
+      <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>12723231.45811424</v>
+        <v>109617373.6895769</v>
       </c>
       <c r="F52" t="n">
-        <v>10513635134.08033</v>
+        <v>89537059870</v>
       </c>
       <c r="G52" t="n">
-        <v>293071.6933015965</v>
+        <v>2487471.73642611</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
       </c>
       <c r="I52" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -2163,28 +2031,26 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Magallanes y Antártica</t>
+          <t>Los Ríos</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>47999471.90551676</v>
+        <v>41389788.17639003</v>
       </c>
       <c r="F53" t="n">
-        <v>42361610244</v>
-      </c>
-      <c r="G53" t="n">
-        <v>1170008.393027822</v>
-      </c>
+        <v>34863311480.4782</v>
+      </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="n">
         <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
@@ -2196,28 +2062,26 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Magallanes y Antártica</t>
+          <t>Los Ríos</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>29869978.09887428</v>
+        <v>29345224.70572385</v>
       </c>
       <c r="F54" t="n">
-        <v>24511161795.44435</v>
-      </c>
-      <c r="G54" t="n">
-        <v>684732.9932172245</v>
-      </c>
+        <v>24827654181.91487</v>
+      </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
         <v>0</v>
       </c>
       <c r="I54" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
@@ -2229,7 +2093,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Magallanes y Antártica</t>
+          <t>Los Ríos</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2238,19 +2102,17 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>15545129.34176308</v>
+        <v>18866703.59299771</v>
       </c>
       <c r="F55" t="n">
-        <v>13197281825.55735</v>
-      </c>
-      <c r="G55" t="n">
-        <v>366567.486918636</v>
-      </c>
+        <v>15664639472.27977</v>
+      </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="n">
         <v>0</v>
       </c>
       <c r="I55" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
@@ -2262,28 +2124,26 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Magallanes y Antártica</t>
+          <t>Los Ríos</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Obras MINVU</t>
+          <t>Salud, servicios sanitarios y alimentación</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>15507357.87048403</v>
+        <v>14083575.58454207</v>
       </c>
       <c r="F56" t="n">
-        <v>13192735078.97734</v>
-      </c>
-      <c r="G56" t="n">
-        <v>364343.720608453</v>
-      </c>
+        <v>11703945947.56422</v>
+      </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="n">
         <v>0</v>
       </c>
       <c r="I56" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57">
@@ -2298,25 +2158,21 @@
           <t>Magallanes y Antártica</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
-        </is>
-      </c>
+      <c r="D57" t="inlineStr"/>
       <c r="E57" t="n">
-        <v>13569111.42519188</v>
+        <v>61379845.62351756</v>
       </c>
       <c r="F57" t="n">
-        <v>11337639241.29451</v>
+        <v>53976679919</v>
       </c>
       <c r="G57" t="n">
-        <v>315583.7900633437</v>
+        <v>1488491.763933692</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -2328,7 +2184,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Maule</t>
+          <t>Magallanes y Antártica</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2337,19 +2193,17 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>68324237.345009</v>
+        <v>33304843.31895265</v>
       </c>
       <c r="F58" t="n">
-        <v>57432213146.10165</v>
-      </c>
-      <c r="G58" t="n">
-        <v>1595466.988736349</v>
-      </c>
+        <v>27507200527.17492</v>
+      </c>
+      <c r="G58" t="inlineStr"/>
       <c r="H58" t="n">
         <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -2361,28 +2215,26 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Maule</t>
+          <t>Magallanes y Antártica</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Obras MINVU</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>59134164.7376148</v>
+        <v>22792563.78664332</v>
       </c>
       <c r="F59" t="n">
-        <v>47982275728</v>
-      </c>
-      <c r="G59" t="n">
-        <v>1330953.977357862</v>
-      </c>
+        <v>19564617769.97734</v>
+      </c>
+      <c r="G59" t="inlineStr"/>
       <c r="H59" t="n">
         <v>0</v>
       </c>
       <c r="I59" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
@@ -2394,28 +2246,26 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Maule</t>
+          <t>Magallanes y Antártica</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>50275088.20098618</v>
+        <v>16649682.38543603</v>
       </c>
       <c r="F60" t="n">
-        <v>42024861104.25966</v>
-      </c>
-      <c r="G60" t="n">
-        <v>1174612.5333055</v>
-      </c>
+        <v>14163299862.91663</v>
+      </c>
+      <c r="G60" t="inlineStr"/>
       <c r="H60" t="n">
         <v>0</v>
       </c>
       <c r="I60" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -2427,28 +2277,26 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Maule</t>
+          <t>Magallanes y Antártica</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>49449202.39645066</v>
+        <v>14623663.32306321</v>
       </c>
       <c r="F61" t="n">
-        <v>41310932561.82267</v>
-      </c>
-      <c r="G61" t="n">
-        <v>1149690.514877998</v>
-      </c>
+        <v>12259828719.89903</v>
+      </c>
+      <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
         <v>0</v>
       </c>
       <c r="I61" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -2465,23 +2313,21 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Obras MINVU</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>42909800.90529323</v>
+        <v>74252566.25951196</v>
       </c>
       <c r="F62" t="n">
-        <v>37436491609.90449</v>
-      </c>
-      <c r="G62" t="n">
-        <v>1031176.87916136</v>
-      </c>
+        <v>62616581647.55495</v>
+      </c>
+      <c r="G62" t="inlineStr"/>
       <c r="H62" t="n">
         <v>0</v>
       </c>
       <c r="I62" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -2493,28 +2339,24 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Metropolitana</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Medicamentos y productos farmacéuticos</t>
-        </is>
-      </c>
+          <t>Maule</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
       <c r="E63" t="n">
-        <v>1170032824.754314</v>
+        <v>60146679.88510414</v>
       </c>
       <c r="F63" t="n">
-        <v>964733831086.9896</v>
+        <v>48828564123</v>
       </c>
       <c r="G63" t="n">
-        <v>26885243.7696996</v>
+        <v>1354604.918297481</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
       </c>
       <c r="I63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -2526,28 +2368,26 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Metropolitana</t>
+          <t>Maule</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Salud, servicios sanitarios y alimentación</t>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>490819798.6794276</v>
+        <v>56465735.1633732</v>
       </c>
       <c r="F64" t="n">
-        <v>411109067807.092</v>
-      </c>
-      <c r="G64" t="n">
-        <v>11454722.61511249</v>
-      </c>
+        <v>47324148844.73659</v>
+      </c>
+      <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
         <v>0</v>
       </c>
       <c r="I64" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65">
@@ -2559,7 +2399,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Metropolitana</t>
+          <t>Maule</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2568,19 +2408,17 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>429533558.8206079</v>
+        <v>53470197.19490345</v>
       </c>
       <c r="F65" t="n">
-        <v>358760608319.3102</v>
-      </c>
-      <c r="G65" t="n">
-        <v>9989530.377153313</v>
-      </c>
+        <v>44827022219.4157</v>
+      </c>
+      <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
         <v>0</v>
       </c>
       <c r="I65" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
@@ -2592,28 +2430,26 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Metropolitana</t>
+          <t>Maule</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Obras MINVU</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>392626642.7708862</v>
+        <v>43726748.89731067</v>
       </c>
       <c r="F66" t="n">
-        <v>316193907103</v>
-      </c>
-      <c r="G66" t="n">
-        <v>8868180.003538791</v>
-      </c>
+        <v>37779561009.98734</v>
+      </c>
+      <c r="G66" t="inlineStr"/>
       <c r="H66" t="n">
         <v>0</v>
       </c>
       <c r="I66" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67">
@@ -2630,23 +2466,21 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Medicamentos y productos farmacéuticos</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>387881646.6223531</v>
+        <v>1245880871.338465</v>
       </c>
       <c r="F67" t="n">
-        <v>323963189844.4384</v>
-      </c>
-      <c r="G67" t="n">
-        <v>9025552.693716351</v>
-      </c>
+        <v>1031082771984.208</v>
+      </c>
+      <c r="G67" t="inlineStr"/>
       <c r="H67" t="n">
         <v>0</v>
       </c>
       <c r="I67" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -2658,28 +2492,24 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Ñuble</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Servicios de construcción y mantenimiento</t>
-        </is>
-      </c>
+          <t>Metropolitana</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>41333397.30786698</v>
+        <v>512794630.8053578</v>
       </c>
       <c r="F68" t="n">
-        <v>34808270310.34961</v>
+        <v>417101963736</v>
       </c>
       <c r="G68" t="n">
-        <v>967947.0989779389</v>
+        <v>11669153.75548899</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
       </c>
       <c r="I68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -2691,28 +2521,26 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Ñuble</t>
+          <t>Metropolitana</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Obras MINVU</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>24344812.84109649</v>
+        <v>449948213.4182352</v>
       </c>
       <c r="F69" t="n">
-        <v>21034990338.02969</v>
-      </c>
-      <c r="G69" t="n">
-        <v>581933.7987256635</v>
-      </c>
+        <v>377021198025.541</v>
+      </c>
+      <c r="G69" t="inlineStr"/>
       <c r="H69" t="n">
         <v>0</v>
       </c>
       <c r="I69" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70">
@@ -2724,28 +2552,26 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Ñuble</t>
+          <t>Metropolitana</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Servicios de transporte, almacenaje y correo</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>20265392.68915411</v>
+        <v>381535217.8998587</v>
       </c>
       <c r="F70" t="n">
-        <v>16928417304.54245</v>
-      </c>
-      <c r="G70" t="n">
-        <v>470648.5513425617</v>
-      </c>
+        <v>323310290829.6418</v>
+      </c>
+      <c r="G70" t="inlineStr"/>
       <c r="H70" t="n">
         <v>0</v>
       </c>
       <c r="I70" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
@@ -2757,28 +2583,26 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Ñuble</t>
+          <t>Metropolitana</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Servicios basados en ingeniería, ciencias sociales y tecnología de la información</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>17477308.45293474</v>
+        <v>351973947.2715064</v>
       </c>
       <c r="F71" t="n">
-        <v>14797455777.15814</v>
-      </c>
-      <c r="G71" t="n">
-        <v>410732.6308136528</v>
-      </c>
+        <v>296273919127.8158</v>
+      </c>
+      <c r="G71" t="inlineStr"/>
       <c r="H71" t="n">
         <v>0</v>
       </c>
       <c r="I71" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72">
@@ -2795,23 +2619,21 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+          <t>Servicios de construcción y mantenimiento</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>17195997.25982706</v>
+        <v>123254360.5859251</v>
       </c>
       <c r="F72" t="n">
-        <v>14310840742.55099</v>
-      </c>
-      <c r="G72" t="n">
-        <v>398606.7979493482</v>
-      </c>
+        <v>101588784520.8411</v>
+      </c>
+      <c r="G72" t="inlineStr"/>
       <c r="H72" t="n">
         <v>0</v>
       </c>
       <c r="I72" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -2823,28 +2645,28 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Tarapacá</t>
+          <t>Ñuble</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Sin Información</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>25809625.98945259</v>
+        <v>24443328.93593493</v>
       </c>
       <c r="F73" t="n">
-        <v>21759558652.5514</v>
+        <v>21140457873.18453</v>
       </c>
       <c r="G73" t="n">
-        <v>605399.4355561425</v>
+        <v>583912.4051245149</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
       </c>
       <c r="I73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
@@ -2856,28 +2678,26 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Tarapacá</t>
+          <t>Ñuble</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Servicios de transporte, almacenaje y correo</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>19821943.13195308</v>
+        <v>22680111.59829282</v>
       </c>
       <c r="F74" t="n">
-        <v>16550571787.31311</v>
-      </c>
-      <c r="G74" t="n">
-        <v>460606.1283392833</v>
-      </c>
+        <v>19035314624.30814</v>
+      </c>
+      <c r="G74" t="inlineStr"/>
       <c r="H74" t="n">
         <v>0</v>
       </c>
       <c r="I74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
@@ -2889,7 +2709,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Tarapacá</t>
+          <t>Ñuble</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2898,19 +2718,17 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>12584808.70373974</v>
+        <v>21972388.90992018</v>
       </c>
       <c r="F75" t="n">
-        <v>10603665118.48442</v>
-      </c>
-      <c r="G75" t="n">
-        <v>294638.2552378968</v>
-      </c>
+        <v>18453049421.75361</v>
+      </c>
+      <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
         <v>0</v>
       </c>
       <c r="I75" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76">
@@ -2922,28 +2740,26 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Tarapacá</t>
+          <t>Ñuble</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Servicios de limpieza industrial</t>
+          <t>Equipamiento y suministros médicos</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>11699710.79084001</v>
+        <v>19379773.17125701</v>
       </c>
       <c r="F76" t="n">
-        <v>9736017953.098408</v>
-      </c>
-      <c r="G76" t="n">
-        <v>271551.7016014787</v>
-      </c>
+        <v>16462359695.295</v>
+      </c>
+      <c r="G76" t="inlineStr"/>
       <c r="H76" t="n">
         <v>0</v>
       </c>
       <c r="I76" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77">
@@ -2955,28 +2771,26 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Tarapacá</t>
+          <t>Sin información</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Servicios de transporte, almacenaje y correo</t>
+          <t>Tecnologías de la información, telecomunicaciones y radiodifusión</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>9181883.901422272</v>
+        <v>5053.726229795701</v>
       </c>
       <c r="F77" t="n">
-        <v>7693146563.492121</v>
-      </c>
-      <c r="G77" t="n">
-        <v>214083.416295578</v>
-      </c>
+        <v>4411800</v>
+      </c>
+      <c r="G77" t="inlineStr"/>
       <c r="H77" t="n">
         <v>0</v>
       </c>
       <c r="I77" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -2988,28 +2802,26 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>Sin información</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Servicios de construcción y mantenimiento</t>
+          <t>Servicios de transporte, almacenaje y correo</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>101011544.1185638</v>
+        <v>4732.721525935397</v>
       </c>
       <c r="F78" t="n">
-        <v>84314692343.75438</v>
-      </c>
-      <c r="G78" t="n">
-        <v>2344531.431942334</v>
-      </c>
+        <v>3919818</v>
+      </c>
+      <c r="G78" t="inlineStr"/>
       <c r="H78" t="n">
         <v>0</v>
       </c>
       <c r="I78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79">
@@ -3021,28 +2833,26 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>Sin información</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Equipamiento y suministros médicos</t>
+          <t>Vehículos y equipamiento en general</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>96151259.3789192</v>
+        <v>4410.956829840198</v>
       </c>
       <c r="F79" t="n">
-        <v>80527465432.23483</v>
-      </c>
-      <c r="G79" t="n">
-        <v>2241269.31622391</v>
-      </c>
+        <v>4089041</v>
+      </c>
+      <c r="G79" t="inlineStr"/>
       <c r="H79" t="n">
         <v>0</v>
       </c>
       <c r="I79" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
@@ -3054,28 +2864,26 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>Sin información</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Obras</t>
+          <t>Medicamentos y productos farmacéuticos</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>78643826.5932968</v>
+        <v>2655.174627710657</v>
       </c>
       <c r="F80" t="n">
-        <v>63424145641</v>
-      </c>
-      <c r="G80" t="n">
-        <v>1773299.927686582</v>
-      </c>
+        <v>2312466</v>
+      </c>
+      <c r="G80" t="inlineStr"/>
       <c r="H80" t="n">
         <v>0</v>
       </c>
       <c r="I80" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
@@ -3087,28 +2895,26 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Valparaíso</t>
+          <t>Sin información</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+          <t>Equipos, accesorios y suministros de oficina</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>74161772.74689664</v>
+        <v>2426.65818972913</v>
       </c>
       <c r="F81" t="n">
-        <v>61255833596.30016</v>
-      </c>
-      <c r="G81" t="n">
-        <v>1710535.350282026</v>
-      </c>
+        <v>2108812</v>
+      </c>
+      <c r="G81" t="inlineStr"/>
       <c r="H81" t="n">
         <v>0</v>
       </c>
       <c r="I81" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -3120,27 +2926,302 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
+          <t>Tarapacá</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Servicios de construcción y mantenimiento</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>29905064.68467002</v>
+      </c>
+      <c r="F82" t="n">
+        <v>25341561096.9814</v>
+      </c>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Tarapacá</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Equipamiento y suministros médicos</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>20863069.25639435</v>
+      </c>
+      <c r="F83" t="n">
+        <v>17460996541.85113</v>
+      </c>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Tarapacá</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>17363264.73087526</v>
+      </c>
+      <c r="F84" t="n">
+        <v>14783044416.01747</v>
+      </c>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Tarapacá</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Servicios de limpieza industrial</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>13231942.77414693</v>
+      </c>
+      <c r="F85" t="n">
+        <v>11076150912.72366</v>
+      </c>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Tarapacá</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Servicios de transporte, almacenaje y correo</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>10425432.63437072</v>
+      </c>
+      <c r="F86" t="n">
+        <v>8780605981.992975</v>
+      </c>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
           <t>Valparaíso</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Servicios de construcción y mantenimiento</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>114031351.5085096</v>
+      </c>
+      <c r="F87" t="n">
+        <v>95629652457.04111</v>
+      </c>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Valparaíso</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Equipamiento y suministros médicos</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>106835103.1967579</v>
+      </c>
+      <c r="F88" t="n">
+        <v>89867292614.95744</v>
+      </c>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Valparaíso</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>82064466.81275922</v>
+      </c>
+      <c r="F89" t="n">
+        <v>66280364260</v>
+      </c>
+      <c r="G89" t="n">
+        <v>1852515.13107252</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Valparaíso</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Servicios profesionales, administrativos y consultorías de gestión empresarial</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>81165262.02298148</v>
+      </c>
+      <c r="F90" t="n">
+        <v>67372669016.7013</v>
+      </c>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>2023</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Valparaíso</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
         <is>
           <t>Servicios de limpieza industrial</t>
         </is>
       </c>
-      <c r="E82" t="n">
-        <v>59170883.07193279</v>
-      </c>
-      <c r="F82" t="n">
-        <v>49124236333.11124</v>
-      </c>
-      <c r="G82" t="n">
-        <v>1368760.573441674</v>
-      </c>
-      <c r="H82" t="n">
-        <v>0</v>
-      </c>
-      <c r="I82" t="n">
+      <c r="E91" t="n">
+        <v>70427948.90482001</v>
+      </c>
+      <c r="F91" t="n">
+        <v>58809972770.20901</v>
+      </c>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>